<commit_message>
Update & new words
</commit_message>
<xml_diff>
--- a/Canciónes/Pochill. Porqué.xlsx
+++ b/Canciónes/Pochill. Porqué.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dropbox\Flashcards Deluxe\Canciónes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ktenzin\Desktop\Español\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22104" windowHeight="11400"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17800" windowHeight="7640"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Text 1</t>
   </si>
@@ -27,85 +27,70 @@
     <t>Text 2</t>
   </si>
   <si>
-    <t>Куда ты уходишь, куда, облако моего одиночества?</t>
-  </si>
-  <si>
-    <t>¿A dónde vas? ¿dónde vas nube de mi soledad?</t>
-  </si>
-  <si>
-    <t>Облако, выливающееся слезами.</t>
-  </si>
-  <si>
-    <t>La nube que no llueve sin lágrimas.</t>
-  </si>
-  <si>
-    <t>Куда ты уходишь, о, мое одиночество?</t>
-  </si>
-  <si>
     <t>¿A dónde vas ahora, oh mi soledad?</t>
   </si>
   <si>
-    <t>Где ты, куда уходишь с моей болью?</t>
-  </si>
-  <si>
     <t>¿A dónde estás, dónde vas con mi dolor?</t>
   </si>
   <si>
-    <t>Почему, почему тебя здесь нет?</t>
-  </si>
-  <si>
-    <t>¿Por qué? ¿Por qué no estás aquí?</t>
-  </si>
-  <si>
-    <t>Эти слова я написала тебе.</t>
-  </si>
-  <si>
-    <t>Son mis palabras, las escribí por ti.</t>
-  </si>
-  <si>
-    <t>Почему? Ведь ты нужна мне,</t>
-  </si>
-  <si>
-    <t>¿Por qué? Porque eres para mí</t>
-  </si>
-  <si>
-    <t>Слушай, я пою тебе эти слова.</t>
-  </si>
-  <si>
-    <t>Oye, Con mis palabras, yo te las canto así.</t>
-  </si>
-  <si>
-    <t>Куда ты уходишь с песнями?</t>
-  </si>
-  <si>
-    <t>¿A dónde vas, como va, con las canciones?</t>
-  </si>
-  <si>
-    <t>С песнями, которые написала для тебя.</t>
-  </si>
-  <si>
-    <t>Las canciones que te escribí</t>
-  </si>
-  <si>
-    <t>Куда ты теперь уходишь, о, мое одиночество?</t>
-  </si>
-  <si>
     <t>Мое одиночество – это ты.</t>
   </si>
   <si>
     <t>¡Mi soledad, soledad eres tú!</t>
   </si>
   <si>
-    <t>Облако больше не плачет,</t>
-  </si>
-  <si>
-    <t>La nube que llovía no llueve más</t>
+    <t>Куда ты уходишь с песнями?
+С песнями, которые написала для тебя.</t>
+  </si>
+  <si>
+    <t>¿A dónde vas, como va, con las canciones?
+Las canciones que te escribí</t>
+  </si>
+  <si>
+    <t>¿Por qué? ¿Por qué no estás aquí?
+Son mis palabras, las escribí por ti.</t>
+  </si>
+  <si>
+    <t>¿Por qué? Porque eres para mí
+Oye, Con mis palabras, yo te las canto así.</t>
+  </si>
+  <si>
+    <t>¿A dónde vas? ¿dónde vas nube de mi soledad?
+La nube que no llueve sin lágrimas.</t>
+  </si>
+  <si>
+    <t>¿A dónde vas? ¿dónde vas nube de mi soledad?
+La nube que llovía no llueve más</t>
+  </si>
+  <si>
+    <t>Куда ты идешь? Где ты, облако моего одиночества
+Облако, из которого не идет дождь, как раньше?</t>
+  </si>
+  <si>
+    <t>Куда ты идешь? Куда идешь,
+Облако моего одиночества,
+Облако, что не проливает дождя без слез?</t>
+  </si>
+  <si>
+    <t>Куда теперь ты идешь, о, мое одиночество?</t>
+  </si>
+  <si>
+    <t>Где ты, куда ты идешь с моей болью?</t>
+  </si>
+  <si>
+    <t>Почему, почему ты не здесь?
+Это мои слова, я написала их для тебя…</t>
+  </si>
+  <si>
+    <t>Почему? Потому что ты – для меня…
+Послушай…
+С моими словами, вот так я их пою для тебя.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -116,10 +101,12 @@
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -152,7 +139,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -168,9 +155,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -208,7 +195,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -280,7 +267,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -436,16 +423,16 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="46" customWidth="1"/>
-    <col min="2" max="2" width="41.109375" customWidth="1"/>
+    <col min="2" max="2" width="41.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -453,110 +440,75 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+    </row>
+    <row r="4" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="5" spans="1:2" ht="25" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="25" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="2" t="s">
+    <row r="9" spans="1:2" ht="25" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
+    <row r="10" spans="1:2" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:2" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:2" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:2" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:2" ht="12.5" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>